<commit_message>
filtered new employee list updated with role and point ids
</commit_message>
<xml_diff>
--- a/formatted_new_employee_list.xlsx
+++ b/formatted_new_employee_list.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18562" uniqueCount="3950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18553" uniqueCount="3950">
   <si>
     <t xml:space="preserve">User Code</t>
   </si>
@@ -68184,7 +68184,7 @@
   <dimension ref="A1:AS192"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -70265,9 +70265,6 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B18" s="0" t="s">
         <v>255</v>
       </c>
@@ -71006,9 +71003,6 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B24" s="0" t="s">
         <v>402</v>
       </c>
@@ -71616,9 +71610,6 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B29" s="0" t="s">
         <v>447</v>
       </c>
@@ -72812,9 +72803,6 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B39" s="0" t="s">
         <v>561</v>
       </c>
@@ -72937,9 +72925,6 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B40" s="0" t="s">
         <v>571</v>
       </c>
@@ -73422,9 +73407,6 @@
       </c>
     </row>
     <row r="44" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="n">
-        <v>0</v>
-      </c>
       <c r="B44" s="8" t="s">
         <v>610</v>
       </c>
@@ -73550,9 +73532,6 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B45" s="0" t="s">
         <v>619</v>
       </c>
@@ -73675,9 +73654,6 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B46" s="0" t="s">
         <v>641</v>
       </c>
@@ -73800,9 +73776,6 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B47" s="0" t="s">
         <v>653</v>
       </c>
@@ -73925,9 +73898,6 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B48" s="0" t="s">
         <v>662</v>
       </c>
@@ -77570,9 +77540,6 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>1016</v>
-      </c>
       <c r="B79" s="0" t="s">
         <v>1017</v>
       </c>
@@ -77683,9 +77650,6 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>1016</v>
-      </c>
       <c r="B80" s="0" t="s">
         <v>1026</v>
       </c>
@@ -77796,9 +77760,6 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>1016</v>
-      </c>
       <c r="B81" s="0" t="s">
         <v>1033</v>
       </c>
@@ -77906,9 +77867,6 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>1016</v>
-      </c>
       <c r="B82" s="0" t="s">
         <v>1041</v>
       </c>
@@ -78022,9 +77980,6 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>1016</v>
-      </c>
       <c r="B83" s="0" t="s">
         <v>1048</v>
       </c>
@@ -78138,9 +78093,6 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>1016</v>
-      </c>
       <c r="B84" s="0" t="s">
         <v>1054</v>
       </c>
@@ -78254,9 +78206,6 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>1016</v>
-      </c>
       <c r="B85" s="0" t="s">
         <v>1063</v>
       </c>
@@ -78376,9 +78325,6 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>1016</v>
-      </c>
       <c r="B86" s="0" t="s">
         <v>1071</v>
       </c>
@@ -78492,9 +78438,6 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>1016</v>
-      </c>
       <c r="B87" s="0" t="s">
         <v>1079</v>
       </c>
@@ -82670,9 +82613,6 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B125" s="0" t="s">
         <v>1676</v>
       </c>
@@ -82795,9 +82735,6 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B126" s="0" t="s">
         <v>1682</v>
       </c>
@@ -84046,9 +83983,6 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B137" s="0" t="s">
         <v>1803</v>
       </c>
@@ -84171,9 +84105,6 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B138" s="0" t="s">
         <v>1813</v>
       </c>
@@ -84395,9 +84326,6 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B140" s="0" t="s">
         <v>1842</v>
       </c>
@@ -84520,9 +84448,6 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B141" s="0" t="s">
         <v>1848</v>
       </c>
@@ -84645,9 +84570,6 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B142" s="0" t="s">
         <v>1856</v>
       </c>
@@ -86758,9 +86680,6 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B160" s="0" t="s">
         <v>3650</v>
       </c>
@@ -88022,9 +87941,6 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B171" s="0" t="s">
         <v>3743</v>
       </c>
@@ -88619,9 +88535,6 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B176" s="0" t="s">
         <v>3784</v>
       </c>
@@ -89574,9 +89487,6 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B184" s="0" t="s">
         <v>3843</v>
       </c>
@@ -89794,9 +89704,6 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B186" s="0" t="s">
         <v>3879</v>
       </c>
@@ -90026,9 +89933,6 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B188" s="0" t="s">
         <v>3898</v>
       </c>
@@ -90151,9 +90055,6 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B189" s="0" t="s">
         <v>3906</v>
       </c>
@@ -90398,9 +90299,6 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B191" s="0" t="s">
         <v>3927</v>
       </c>

</xml_diff>